<commit_message>
Arreglo el cableado de corriente en el informe. Coloco los arreglos en el cableado de corriente en PRESUPUESTO.xlsx y quito PRESUPUESTOX.xlsx.
</commit_message>
<xml_diff>
--- a/CABLEADO ESTRUCTURADO/PRESUPUESTO.xlsx
+++ b/CABLEADO ESTRUCTURADO/PRESUPUESTO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="8760" yWindow="-120" windowWidth="10275" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="73">
   <si>
     <t>Piso:</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Tablero general</t>
   </si>
   <si>
-    <t>Termica</t>
-  </si>
-  <si>
     <t>Disyuntor</t>
   </si>
   <si>
@@ -168,30 +165,18 @@
     <t>Roseta</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2 x piso</t>
-  </si>
-  <si>
-    <t>1  x PC</t>
-  </si>
-  <si>
     <t>Metros UTP Total:</t>
   </si>
   <si>
     <t>Configuración de equipos puesto de trabajo</t>
   </si>
   <si>
-    <t>Cable entrada corriente 8,25mm</t>
-  </si>
-  <si>
     <t>cable electrico grueso</t>
   </si>
   <si>
     <t>fino</t>
   </si>
   <si>
-    <t>pb</t>
-  </si>
-  <si>
     <t>cable/piso</t>
   </si>
   <si>
@@ -211,6 +196,48 @@
   </si>
   <si>
     <t>Costo</t>
+  </si>
+  <si>
+    <t>pb(10mm)</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>pb entrada10mm</t>
+  </si>
+  <si>
+    <t>pb grueso 4mm</t>
+  </si>
+  <si>
+    <t>1 grueso 4mm</t>
+  </si>
+  <si>
+    <t>2 grueso 4mm</t>
+  </si>
+  <si>
+    <t>3 grueso 4mm</t>
+  </si>
+  <si>
+    <t>4 grueso 4mm</t>
+  </si>
+  <si>
+    <t>5 grueso 4mm</t>
+  </si>
+  <si>
+    <t>1s grueso 1,5mm</t>
+  </si>
+  <si>
+    <t>2sgrueso 1,5mm</t>
+  </si>
+  <si>
+    <t>exp grueso 1,5mm</t>
+  </si>
+  <si>
+    <t>fino 1,5 mm</t>
+  </si>
+  <si>
+    <t>total real</t>
   </si>
 </sst>
 </file>
@@ -220,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +337,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,13 +443,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -526,20 +558,13 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,7 +574,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -852,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N112"/>
+  <dimension ref="A3:O112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O115" sqref="O115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,27 +908,27 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E3" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
+      <c r="E3" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1064,7 +1096,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10">
         <v>1</v>
@@ -1078,7 +1110,7 @@
       </c>
       <c r="F14" s="23"/>
       <c r="I14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="10">
         <v>1</v>
@@ -1093,7 +1125,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="10">
         <v>6</v>
@@ -1107,7 +1139,7 @@
       </c>
       <c r="F15" s="23"/>
       <c r="I15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="10">
         <v>6</v>
@@ -1122,7 +1154,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -1133,7 +1165,7 @@
       </c>
       <c r="F16" s="29"/>
       <c r="H16" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="33"/>
       <c r="J16" s="33"/>
@@ -1283,7 +1315,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1312,7 +1344,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -1413,7 +1445,7 @@
       </c>
       <c r="F30" s="23"/>
       <c r="I30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" s="22">
         <v>5</v>
@@ -1442,7 +1474,7 @@
       </c>
       <c r="F31" s="23"/>
       <c r="I31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J31" s="10">
         <v>84</v>
@@ -1471,7 +1503,7 @@
       </c>
       <c r="F32" s="23"/>
       <c r="I32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J32" s="10">
         <v>15</v>
@@ -1500,7 +1532,7 @@
       </c>
       <c r="F33" s="23"/>
       <c r="H33" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I33" s="33"/>
       <c r="J33" s="33"/>
@@ -1512,7 +1544,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="22">
         <v>3</v>
@@ -1530,7 +1562,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="10">
         <v>40</v>
@@ -1547,7 +1579,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="22">
         <v>1</v>
@@ -1566,7 +1598,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
@@ -1793,7 +1825,7 @@
       </c>
       <c r="F47" s="27"/>
       <c r="I47" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47" s="22">
         <v>1</v>
@@ -1822,7 +1854,7 @@
       </c>
       <c r="F48" s="27"/>
       <c r="I48" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J48" s="22">
         <v>6</v>
@@ -1851,7 +1883,7 @@
       </c>
       <c r="F49" s="23"/>
       <c r="I49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J49" s="10">
         <v>84</v>
@@ -1866,7 +1898,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C50" s="10">
         <v>4</v>
@@ -1879,7 +1911,7 @@
         <v>48</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J50" s="10">
         <v>20</v>
@@ -1894,7 +1926,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C51" s="10">
         <v>56</v>
@@ -1907,7 +1939,7 @@
         <v>728</v>
       </c>
       <c r="H51" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I51" s="33"/>
       <c r="J51" s="33"/>
@@ -1920,7 +1952,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" s="10">
         <v>18</v>
@@ -1938,7 +1970,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
@@ -2185,7 +2217,7 @@
       </c>
       <c r="F64" s="30"/>
       <c r="I64" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J64" s="22">
         <v>1</v>
@@ -2198,7 +2230,7 @@
         <v>3935</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>19</v>
       </c>
@@ -2213,7 +2245,7 @@
         <v>1190</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J65" s="22">
         <v>2</v>
@@ -2226,9 +2258,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C66" s="22">
         <v>4</v>
@@ -2243,7 +2275,7 @@
       <c r="F66" s="6"/>
       <c r="H66" s="12"/>
       <c r="I66" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J66" s="25">
         <v>28</v>
@@ -2256,9 +2288,9 @@
         <v>364</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C67" s="10">
         <v>56</v>
@@ -2273,7 +2305,7 @@
       <c r="F67" s="23"/>
       <c r="H67" s="12"/>
       <c r="I67" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J67" s="10">
         <v>28</v>
@@ -2286,9 +2318,9 @@
         <v>420</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" s="10">
         <v>24</v>
@@ -2302,7 +2334,7 @@
       </c>
       <c r="F68" s="27"/>
       <c r="H68" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I68" s="33"/>
       <c r="J68" s="33"/>
@@ -2312,9 +2344,9 @@
         <v>21576.85</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B69" s="33"/>
       <c r="C69" s="33"/>
@@ -2328,35 +2360,35 @@
       <c r="K69" s="34"/>
       <c r="L69" s="34"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D70" s="34"/>
       <c r="E70" s="34"/>
       <c r="F70" s="27"/>
       <c r="K70" s="34"/>
       <c r="L70" s="34"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D71" s="34"/>
       <c r="E71" s="34"/>
       <c r="F71" s="27"/>
       <c r="K71" s="34"/>
       <c r="L71" s="34"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D72" s="34"/>
       <c r="E72" s="34"/>
       <c r="F72" s="23"/>
       <c r="K72" s="34"/>
       <c r="L72" s="34"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D73" s="34"/>
       <c r="E73" s="34"/>
       <c r="F73" s="23"/>
       <c r="K73" s="34"/>
       <c r="L73" s="34"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D74" s="34"/>
       <c r="E74" s="34"/>
       <c r="F74" s="23"/>
@@ -2367,7 +2399,7 @@
       <c r="K74" s="34"/>
       <c r="L74" s="34"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -2390,7 +2422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>2</v>
       </c>
@@ -2416,11 +2448,8 @@
         <f t="shared" ref="L76:L81" si="15">J76*K76</f>
         <v>1300</v>
       </c>
-      <c r="M76" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
@@ -2438,17 +2467,17 @@
         <v>28</v>
       </c>
       <c r="J77" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K77" s="42">
         <v>20000</v>
       </c>
       <c r="L77" s="42">
         <f t="shared" si="15"/>
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
@@ -2476,7 +2505,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>18</v>
       </c>
@@ -2494,18 +2523,17 @@
         <v>33</v>
       </c>
       <c r="J79" s="10">
-        <f>C14+J14+J30+C34+C50+J48+C66+J65+C82</f>
-        <v>27</v>
-      </c>
-      <c r="K79" s="42">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="K79" s="43">
+        <v>60</v>
       </c>
       <c r="L79" s="42">
-        <f t="shared" si="15"/>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+        <f>J79*K79</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>21</v>
       </c>
@@ -2520,17 +2548,18 @@
         <v>21.849999999999998</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="J80" s="10">
-        <v>7</v>
+        <v>47</v>
+      </c>
+      <c r="J80" s="47">
+        <f>C25+C33+J25+C45+J42+C61+J59+C78</f>
+        <v>88</v>
       </c>
       <c r="K80" s="43">
-        <v>60</v>
-      </c>
-      <c r="L80" s="42">
-        <f t="shared" si="15"/>
-        <v>420</v>
+        <v>30</v>
+      </c>
+      <c r="L80" s="43">
+        <f>J80*K80</f>
+        <v>2640</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -2547,27 +2576,20 @@
         <f>D81*C81</f>
         <v>195</v>
       </c>
-      <c r="I81" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J81" s="50">
-        <f>C25+C33+J25+C45+J42+C61+J59+C78</f>
-        <v>88</v>
-      </c>
-      <c r="K81" s="43">
-        <v>30</v>
-      </c>
-      <c r="L81" s="43">
-        <f t="shared" si="15"/>
-        <v>2640</v>
-      </c>
-      <c r="M81" t="s">
-        <v>50</v>
+      <c r="H81" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I81" s="33"/>
+      <c r="J81" s="33"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="41">
+        <f>SUM(L76:L80)</f>
+        <v>25760</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C82" s="22">
         <v>1</v>
@@ -2579,23 +2601,14 @@
         <f>D82*C82</f>
         <v>12</v>
       </c>
-      <c r="I82" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="J82" s="48">
-        <v>20</v>
-      </c>
-      <c r="K82" s="49">
-        <v>6.5</v>
-      </c>
-      <c r="L82" s="49">
-        <f>K82*J82</f>
-        <v>130</v>
-      </c>
+      <c r="I82" s="53"/>
+      <c r="J82" s="54"/>
+      <c r="L82" s="55"/>
+      <c r="M82" s="11"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C83" s="10">
         <v>8</v>
@@ -2607,20 +2620,10 @@
         <f>D83*C83</f>
         <v>104</v>
       </c>
-      <c r="H83" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="I83" s="33"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="41">
-        <f>SUM(L76:L82)</f>
-        <v>46214</v>
-      </c>
     </row>
     <row r="84" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84" s="33"/>
       <c r="C84" s="33"/>
@@ -2637,7 +2640,7 @@
     </row>
     <row r="86" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I86" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J86" s="16">
         <f>C83+J66+C67+J49+J31+C35+J15+C15</f>
@@ -2646,7 +2649,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I87" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J87">
         <v>13</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C88">
         <f>C13+J13+C30+J28+C48+J62+C64+J45+C80-37.2</f>
@@ -2663,7 +2666,7 @@
       <c r="D88" s="42">
         <v>0.95</v>
       </c>
-      <c r="E88" s="56">
+      <c r="E88" s="49">
         <f>C88*D88</f>
         <v>2387.16</v>
       </c>
@@ -2673,12 +2676,12 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F94" s="55" t="s">
+      <c r="F94" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="G94" s="55"/>
-      <c r="H94" s="55"/>
-      <c r="I94" s="55"/>
+      <c r="G94" s="52"/>
+      <c r="H94" s="52"/>
+      <c r="I94" s="52"/>
     </row>
     <row r="95" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="F95" s="15"/>
@@ -2688,12 +2691,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F97" s="14"/>
     </row>
-    <row r="98" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F98" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G98" s="16"/>
       <c r="H98" s="16"/>
@@ -2701,7 +2704,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="99" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F99" s="37" t="s">
         <v>15</v>
       </c>
@@ -2711,9 +2714,9 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="100" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F100" s="37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G100" s="16"/>
       <c r="H100" s="16"/>
@@ -2721,125 +2724,122 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="101" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F101" s="37" t="s">
         <v>16</v>
       </c>
       <c r="G101" s="16"/>
       <c r="H101" s="16"/>
       <c r="I101" s="36">
-        <f>E84+L83+L68+E69+L51+E53+L33+E37+L16+E16+N109</f>
-        <v>269510.88500000001</v>
-      </c>
-    </row>
-    <row r="102" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+        <f>E84+L81+L68+E69+L51+E53+L33+E37+L16+E16+N110</f>
+        <v>246884.48620000001</v>
+      </c>
+    </row>
+    <row r="102" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F102" s="37"/>
       <c r="G102" s="16"/>
       <c r="H102" s="16"/>
       <c r="I102" s="35"/>
     </row>
-    <row r="103" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F103" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G103" s="16"/>
       <c r="H103" s="16"/>
       <c r="I103" s="35">
         <f>SUM(I98:I102)</f>
-        <v>277510.88500000001</v>
-      </c>
-    </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B106" s="51" t="s">
+        <v>254884.48620000001</v>
+      </c>
+    </row>
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B106" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C106" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D106" s="48">
+        <v>1</v>
+      </c>
+      <c r="E106" s="48">
+        <v>2</v>
+      </c>
+      <c r="F106" s="48">
+        <v>3</v>
+      </c>
+      <c r="G106" s="48">
+        <v>4</v>
+      </c>
+      <c r="H106" s="48">
+        <v>5</v>
+      </c>
+      <c r="I106" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="J106" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="K106" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="L106" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="M106" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C106" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D106" s="51">
-        <v>1</v>
-      </c>
-      <c r="E106" s="51">
-        <v>2</v>
-      </c>
-      <c r="F106" s="51">
-        <v>3</v>
-      </c>
-      <c r="G106" s="51">
-        <v>4</v>
-      </c>
-      <c r="H106" s="51">
-        <v>5</v>
-      </c>
-      <c r="I106" s="51" t="s">
+      <c r="N106" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="J106" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="K106" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="L106" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="M106" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="N106" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B107" s="51" t="s">
-        <v>54</v>
+    </row>
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B107" s="48" t="s">
+        <v>50</v>
       </c>
       <c r="C107" s="10">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D107" s="10">
-        <v>4.5</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="E107" s="10">
-        <v>4.5</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="F107" s="10">
-        <v>4.5</v>
+        <v>12.05</v>
       </c>
       <c r="G107" s="10">
-        <v>4.5</v>
+        <v>15.9</v>
       </c>
       <c r="H107" s="10">
-        <v>4.5</v>
+        <v>19.2</v>
       </c>
       <c r="I107" s="10">
-        <v>4.5</v>
+        <v>3.7</v>
       </c>
       <c r="J107" s="10">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="K107" s="10">
         <v>15</v>
       </c>
-      <c r="L107" s="10">
-        <f>SUM(C107:K107)</f>
-        <v>66.5</v>
-      </c>
+      <c r="L107" s="10"/>
       <c r="M107" s="17">
-        <f>1.5*5</f>
-        <v>7.5</v>
+        <f>1.5*6</f>
+        <v>9</v>
       </c>
       <c r="N107" s="17">
-        <f>M107*(L107+L107*0.1)</f>
-        <v>548.625</v>
-      </c>
-    </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B108" s="51" t="s">
-        <v>55</v>
+        <f>M107*(C107+C107*0.1)</f>
+        <v>217.79999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B108" s="48" t="s">
+        <v>51</v>
       </c>
       <c r="C108" s="10">
-        <v>50.4</v>
+        <v>62.4</v>
       </c>
       <c r="D108" s="10">
         <v>326</v>
@@ -2867,40 +2867,103 @@
       </c>
       <c r="L108" s="10">
         <f>SUM(C108:K108)</f>
-        <v>1065.2999999999997</v>
+        <v>1077.3</v>
       </c>
       <c r="M108" s="17"/>
       <c r="N108" s="17">
-        <f>F110+G110</f>
-        <v>2520.7600000000002</v>
-      </c>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
+        <f>L108*0.55</f>
+        <v>592.51499999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F109">
-        <f>0.24*5</f>
-        <v>1.2</v>
-      </c>
-      <c r="G109">
-        <f>0.56*5</f>
-        <v>2.8000000000000003</v>
+        <f>0.24*6</f>
+        <v>1.44</v>
       </c>
       <c r="N109">
-        <f>N107+N108</f>
-        <v>3069.3850000000002</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
+        <f>SUM(H107:K107)*0.55 +F110</f>
+        <v>86.671199999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F110">
-        <f>F109*(SUM(H108:K108)+C108)</f>
-        <v>346.56</v>
-      </c>
-      <c r="G110">
-        <f>G109*SUM(D108:G108)</f>
-        <v>2174.2000000000003</v>
-      </c>
-    </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E112" s="52"/>
+        <f>F109*(SUM(D107:G107)+2)</f>
+        <v>62.251200000000004</v>
+      </c>
+      <c r="M110" t="s">
+        <v>60</v>
+      </c>
+      <c r="N110">
+        <f>SUM(N107:N109)</f>
+        <v>896.98619999999994</v>
+      </c>
+    </row>
+    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>61</v>
+      </c>
+      <c r="C111" t="s">
+        <v>62</v>
+      </c>
+      <c r="D111" t="s">
+        <v>63</v>
+      </c>
+      <c r="E111" t="s">
+        <v>64</v>
+      </c>
+      <c r="F111" t="s">
+        <v>65</v>
+      </c>
+      <c r="G111" t="s">
+        <v>66</v>
+      </c>
+      <c r="H111" t="s">
+        <v>67</v>
+      </c>
+      <c r="I111" t="s">
+        <v>68</v>
+      </c>
+      <c r="J111" t="s">
+        <v>69</v>
+      </c>
+      <c r="K111" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>71</v>
+      </c>
+      <c r="D112" t="s">
+        <v>71</v>
+      </c>
+      <c r="E112" t="s">
+        <v>71</v>
+      </c>
+      <c r="F112" t="s">
+        <v>71</v>
+      </c>
+      <c r="G112" t="s">
+        <v>71</v>
+      </c>
+      <c r="H112" t="s">
+        <v>71</v>
+      </c>
+      <c r="I112" t="s">
+        <v>71</v>
+      </c>
+      <c r="J112" t="s">
+        <v>71</v>
+      </c>
+      <c r="K112" t="s">
+        <v>71</v>
+      </c>
+      <c r="N112" s="56">
+        <v>652.1</v>
+      </c>
+      <c r="O112" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>